<commit_message>
Added jumper pins to bom. To realize GND isolation, fixed chiller alarm circuit. And fixed silk.
</commit_message>
<xml_diff>
--- a/CoolingBoxWireOrganizer_bom.xlsx
+++ b/CoolingBoxWireOrganizer_bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/CoolingBoxWireOrganizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kitanoitaru/Desktop/M1/CoolingBoxWireOrganizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64573B83-580E-E448-9277-83164A84C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA1848A-E212-5641-9566-97C4E2EF4870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36420" yWindow="780" windowWidth="30780" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="201">
   <si>
     <t>Reference</t>
   </si>
@@ -747,6 +747,21 @@
     <rPh sb="0" eb="4">
       <t>キュウシュウ</t>
     </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>jumper pin</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/ja/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax%20Shopping_Product_Low%20Volume&amp;utm_term=&amp;productid=2618262&amp;utm_content=&amp;utm_id=go_cmp-20195885710_adg-_ad-__dev-c_ext-_prd-2618262_sig-Cj0KCQjw4Oe4BhCcARIsADQ0csk3KptAQwxkMAcxWVRj6vIKIykWTCykGRXLARAGUXBFWDuMXgmAPkkaAsstEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw4Oe4BhCcARIsADQ0csk3KptAQwxkMAcxWVRj6vIKIykWTCykGRXLARAGUXBFWDuMXgmAPkkaAsstEALw_wcB</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://s3.amazonaws.com/catalogspreads-pdf/PAGE128-129%20.100%20JUMPER.pdf</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1752,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="89" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2701,9 +2716,27 @@
       </c>
     </row>
     <row r="37" spans="3:10">
+      <c r="C37" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F37" t="s">
+        <v>197</v>
+      </c>
+      <c r="G37" t="s">
+        <v>198</v>
+      </c>
+      <c r="H37">
+        <v>16</v>
+      </c>
       <c r="I37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="3:10">
@@ -3017,7 +3050,7 @@
       </c>
       <c r="I57" s="4">
         <f>SUM(I2:I56)</f>
-        <v>65024</v>
+        <v>65056</v>
       </c>
     </row>
   </sheetData>
@@ -3078,6 +3111,8 @@
     <hyperlink ref="E36" r:id="rId50" xr:uid="{0EFE1CFD-3899-4545-95EB-5F532D993A0E}"/>
     <hyperlink ref="C29" r:id="rId51" xr:uid="{DBB7A5C1-EFCA-7C4E-93EA-841FA1D2CCEA}"/>
     <hyperlink ref="E49" r:id="rId52" xr:uid="{4F5184F6-E1B2-804C-92DE-E2E074A050D8}"/>
+    <hyperlink ref="E37" r:id="rId53" display="https://www.digikey.jp/ja/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262?utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax%20Shopping_Product_Low%20Volume&amp;utm_term=&amp;productid=2618262&amp;utm_content=&amp;utm_id=go_cmp-20195885710_adg-_ad-__dev-c_ext-_prd-2618262_sig-Cj0KCQjw4Oe4BhCcARIsADQ0csk3KptAQwxkMAcxWVRj6vIKIykWTCykGRXLARAGUXBFWDuMXgmAPkkaAsstEALw_wcB&amp;gad_source=1&amp;gclid=Cj0KCQjw4Oe4BhCcARIsADQ0csk3KptAQwxkMAcxWVRj6vIKIykWTCykGRXLARAGUXBFWDuMXgmAPkkaAsstEALw_wcB" xr:uid="{625B7CB5-85B1-7C47-960C-134E096DFF79}"/>
+    <hyperlink ref="C37" r:id="rId54" xr:uid="{35F3C887-53A6-974E-A0B4-D8A3F1875299}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>